<commit_message>
Changed normalization to only include first 15 seconds
</commit_message>
<xml_diff>
--- a/Refined Program/rep1_data_analysis/Rep1_DutyRatio_and_AUC.xlsx
+++ b/Refined Program/rep1_data_analysis/Rep1_DutyRatio_and_AUC.xlsx
@@ -486,10 +486,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4706.671673665354</v>
+        <v>4773.971207788346</v>
       </c>
       <c r="G2" t="n">
-        <v>4709.768564787128</v>
+        <v>4777.112380590292</v>
       </c>
     </row>
     <row r="3">
@@ -513,10 +513,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>4065.146143336989</v>
+        <v>3987.239464740323</v>
       </c>
       <c r="G3" t="n">
-        <v>4068.536153259141</v>
+        <v>3990.564506662769</v>
       </c>
     </row>
     <row r="4">
@@ -540,10 +540,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>4134.060585937637</v>
+        <v>4055.418951690293</v>
       </c>
       <c r="G4" t="n">
-        <v>4137.714064941545</v>
+        <v>4059.002931093609</v>
       </c>
     </row>
     <row r="5">
@@ -567,10 +567,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3909.320982646987</v>
+        <v>3933.168334034614</v>
       </c>
       <c r="G5" t="n">
-        <v>3911.852365147509</v>
+        <v>3935.715158287871</v>
       </c>
     </row>
     <row r="6">
@@ -594,10 +594,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5401.098785714421</v>
+        <v>5414.516684202974</v>
       </c>
       <c r="G6" t="n">
-        <v>5405.03126275524</v>
+        <v>5418.458930659206</v>
       </c>
     </row>
     <row r="7">
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3601.161649228945</v>
+        <v>3597.759096711617</v>
       </c>
       <c r="G7" t="n">
-        <v>3604.367725754697</v>
+        <v>3600.962143980478</v>
       </c>
     </row>
     <row r="8">
@@ -675,10 +675,10 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3822.824714754299</v>
+        <v>3891.078051059782</v>
       </c>
       <c r="G9" t="n">
-        <v>3825.420552869055</v>
+        <v>3893.720235691846</v>
       </c>
     </row>
     <row r="10">
@@ -702,10 +702,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3563.345551715164</v>
+        <v>3657.680846070072</v>
       </c>
       <c r="G10" t="n">
-        <v>3565.976009705062</v>
+        <v>3660.380942276402</v>
       </c>
     </row>
     <row r="11">
@@ -729,10 +729,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>3385.166626262809</v>
+        <v>3440.132937663493</v>
       </c>
       <c r="G11" t="n">
-        <v>3387.82333838402</v>
+        <v>3442.832787887457</v>
       </c>
     </row>
     <row r="12">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>4177.181712280423</v>
+        <v>4267.345420107421</v>
       </c>
       <c r="G12" t="n">
-        <v>4178.985199943499</v>
+        <v>4269.187835723823</v>
       </c>
     </row>
     <row r="13">
@@ -783,10 +783,10 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>3717.976297524723</v>
+        <v>3789.952202197283</v>
       </c>
       <c r="G13" t="n">
-        <v>3720.784937760606</v>
+        <v>3792.815214598481</v>
       </c>
     </row>
     <row r="14">
@@ -810,10 +810,10 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1933.80038635018</v>
+        <v>2012.556666321642</v>
       </c>
       <c r="G14" t="n">
-        <v>1933.83671884338</v>
+        <v>2012.594478498077</v>
       </c>
     </row>
     <row r="15">
@@ -837,10 +837,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2631.382239072405</v>
+        <v>2589.229308755906</v>
       </c>
       <c r="G15" t="n">
-        <v>2632.407062332888</v>
+        <v>2590.23771505391</v>
       </c>
     </row>
     <row r="16">
@@ -864,10 +864,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>1997.010217871915</v>
+        <v>2021.262818792059</v>
       </c>
       <c r="G16" t="n">
-        <v>1998.356126460484</v>
+        <v>2022.625072707048</v>
       </c>
     </row>
     <row r="17">
@@ -891,10 +891,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>2889.037083333498</v>
+        <v>2766.519778841928</v>
       </c>
       <c r="G17" t="n">
-        <v>2890.686666666829</v>
+        <v>2768.099407204899</v>
       </c>
     </row>
     <row r="18">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>2364.765532787014</v>
+        <v>2409.801161042567</v>
       </c>
       <c r="G18" t="n">
-        <v>2366.092377049312</v>
+        <v>2411.15327430685</v>
       </c>
     </row>
     <row r="19">
@@ -945,10 +945,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>2411.546547325334</v>
+        <v>2409.678313636498</v>
       </c>
       <c r="G19" t="n">
-        <v>2412.196408818825</v>
+        <v>2410.327671679977</v>
       </c>
     </row>
     <row r="20">
@@ -972,10 +972,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>2583.164522058743</v>
+        <v>2618.927183173505</v>
       </c>
       <c r="G20" t="n">
-        <v>2590.451617646977</v>
+        <v>2626.31516506914</v>
       </c>
     </row>
     <row r="21">
@@ -999,10 +999,10 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>2830.537948717858</v>
+        <v>2968.776355421598</v>
       </c>
       <c r="G21" t="n">
-        <v>2834.721794871705</v>
+        <v>2973.164533132437</v>
       </c>
     </row>
     <row r="22">
@@ -1026,10 +1026,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>2690.055516842021</v>
+        <v>2797.233735770491</v>
       </c>
       <c r="G22" t="n">
-        <v>2695.036700263074</v>
+        <v>2802.413381403152</v>
       </c>
     </row>
     <row r="23">
@@ -1053,10 +1053,10 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2903.516319298157</v>
+        <v>2697.203882007739</v>
       </c>
       <c r="G23" t="n">
-        <v>2909.866363157803</v>
+        <v>2703.102716753501</v>
       </c>
     </row>
     <row r="24">
@@ -1080,10 +1080,10 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>2940.415381689308</v>
+        <v>2888.137963153737</v>
       </c>
       <c r="G24" t="n">
-        <v>2945.680990293716</v>
+        <v>2893.309954908437</v>
       </c>
     </row>
     <row r="25">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>3113.198293055302</v>
+        <v>3105.748039102325</v>
       </c>
       <c r="G25" t="n">
-        <v>3117.990414359976</v>
+        <v>3110.528692290507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>